<commit_message>
Rename of pom objects in common_SD_java classes Excel utility added for python editor Allure reports added Extent reports added
</commit_message>
<xml_diff>
--- a/DSalgoCucumberProj/src/test/resources/Utlils/Python.xlsx
+++ b/DSalgoCucumberProj/src/test/resources/Utlils/Python.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\eclipse-workspace\SampleDSalgo\src\test\resources\Utlils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavit\git\project\DsAlgoCucumberProject\DSalgoCucumberProj\src\test\resources\Utlils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F70D793-DF8A-4BAF-8ACC-5ACE896491AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D5AC0B-BE3C-4619-A32A-37D0D3239FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FF80413-38D8-4CE1-B3DB-07C7AD1BCA43}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>print('Hello, world!')</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78B23A6-BCF3-4484-8A26-3C6085EA4EA2}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -453,6 +456,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>